<commit_message>
v1.0.3 - Versión final
</commit_message>
<xml_diff>
--- a/Data/FicheroEmpleados/USUARIOS.xlsx
+++ b/Data/FicheroEmpleados/USUARIOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup.sharepoint.com/sites/IBERICAN_FCI/Shared Documents/2. Documentación y procesos/12. Procesos automatizados/Liquidación gastos de viaje/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup-my.sharepoint.com/personal/roboticprocessautomation_rpa1_stihl_es/Documents/Documents/UiPath/STIHL_GV_RT1_03_GastosDeViaje/Data/FicheroEmpleados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC104856B11F6C7C5ADE5903" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05101BA2-B6B1-4294-AF62-0E0EA8D638D3}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC104856B11F6C7C5ADE5903" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8265EB1E-C341-44CB-A65A-D5AA8D9A5672}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3300" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,156 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Empleado - Identificador</t>
   </si>
   <si>
     <t>Mail</t>
-  </si>
-  <si>
-    <t>ISMAEL_ASENJO</t>
-  </si>
-  <si>
-    <t>ismael.asenjo@stihl.es</t>
-  </si>
-  <si>
-    <t>ALTAMIRA</t>
-  </si>
-  <si>
-    <t>inaki.altamira@stihl.es</t>
-  </si>
-  <si>
-    <t>ORIOL_PINA</t>
-  </si>
-  <si>
-    <t>oriol.pina@stihl.es</t>
-  </si>
-  <si>
-    <t>TERESA_NIETO</t>
-  </si>
-  <si>
-    <t>teresa.nieto@stihl.es</t>
-  </si>
-  <si>
-    <t>BEGONA_RUIZ</t>
-  </si>
-  <si>
-    <t>begona.ruiz@stihl.es</t>
-  </si>
-  <si>
-    <t>ADOLFOCASASEMPERE</t>
-  </si>
-  <si>
-    <t>adolfo.casasempereblanquer@stihl.es</t>
-  </si>
-  <si>
-    <t>BERND_HULLERUM</t>
-  </si>
-  <si>
-    <t>bernd.hullerum@stihl.es</t>
-  </si>
-  <si>
-    <t>M_MARTINEZ</t>
-  </si>
-  <si>
-    <t>m.martinez@stihl.es</t>
-  </si>
-  <si>
-    <t>MARIO_BALTANAS</t>
-  </si>
-  <si>
-    <t>mario.baltanas@stihl.es</t>
-  </si>
-  <si>
-    <t>PEDRO_MOYANO</t>
-  </si>
-  <si>
-    <t>pedro.moyano@stihl.es</t>
-  </si>
-  <si>
-    <t>FERNANDO_BARRIO</t>
-  </si>
-  <si>
-    <t>fernando.barrio@stihl.es</t>
-  </si>
-  <si>
-    <t>BENJAMIN_MACKH</t>
-  </si>
-  <si>
-    <t>benjamin.mackh@stihl.es</t>
-  </si>
-  <si>
-    <t>ALVARO_LOPEZ</t>
-  </si>
-  <si>
-    <t>alvaro.lopez@stihl.es</t>
-  </si>
-  <si>
-    <t>ANA_SANCHEZ</t>
-  </si>
-  <si>
-    <t>ana.sanchez@stihl.es</t>
-  </si>
-  <si>
-    <t>ENRIQUE_ALONSO</t>
-  </si>
-  <si>
-    <t>enrique.alonso@stihl.es</t>
-  </si>
-  <si>
-    <t>ARANCHA_GANAN</t>
-  </si>
-  <si>
-    <t>arancha.ganan@stihl.es</t>
-  </si>
-  <si>
-    <t>JORGE_HEVIA</t>
-  </si>
-  <si>
-    <t>jorge.hevia@stihl.es</t>
-  </si>
-  <si>
-    <t>VICTOR_PRADA</t>
-  </si>
-  <si>
-    <t>victor.prada@stihl.es</t>
-  </si>
-  <si>
-    <t>RAQUEL_MUNOZ</t>
-  </si>
-  <si>
-    <t>raquel.munoz@stihl.es</t>
-  </si>
-  <si>
-    <t>JSANCHEZ</t>
-  </si>
-  <si>
-    <t>jsanchez@stihl.es</t>
-  </si>
-  <si>
-    <t>JOAQUIN_PORTILLO</t>
-  </si>
-  <si>
-    <t>joaquin.portillo@stihl.es</t>
-  </si>
-  <si>
-    <t>FERNANDO_ALVARO</t>
-  </si>
-  <si>
-    <t>fernando.alvarocastillo@stihl.es</t>
-  </si>
-  <si>
-    <t>ANDRES_LOPEZ</t>
-  </si>
-  <si>
-    <t>andres.lopez@stihl.es</t>
-  </si>
-  <si>
-    <t>JAVIER_SICILIA</t>
-  </si>
-  <si>
-    <t>javier.sicilia@stihl.es</t>
   </si>
   <si>
     <t>TONY_BLANCO</t>
@@ -198,7 +54,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +100,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,19 +369,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,204 +389,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -738,24 +406,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100812FB67C5E01F547A18D4A5FD6A8713D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9642c6788bad27e02d635fb107c9ae4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xmlns:ns3="d9b07192-7579-4291-b28e-58bbe42d995f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e8472eb4e8570153d151932821fc84c" ns2:_="" ns3:_="">
     <xsd:import namespace="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
@@ -990,6 +640,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1000,13 +668,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C25B787B-7428-43A6-BF3C-2BA84D875745}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB358B33-21B5-44C6-8F12-C25C4054C5B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB358B33-21B5-44C6-8F12-C25C4054C5B3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C25B787B-7428-43A6-BF3C-2BA84D875745}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
+    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA831405-C37E-4AB9-AE22-2A9B47C9BFD1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA831405-C37E-4AB9-AE22-2A9B47C9BFD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
v1.0.9 - Cambio selectores descarga fichero SP
</commit_message>
<xml_diff>
--- a/Data/FicheroEmpleados/USUARIOS.xlsx
+++ b/Data/FicheroEmpleados/USUARIOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28712"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup-my.sharepoint.com/personal/roboticprocessautomation_rpa1_stihl_es/Documents/Documents/UiPath/STIHL_GV_RT1_03_GastosDeViaje/Data/FicheroEmpleados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stihlgroup.sharepoint.com/sites/IBERICAN_FCI/Shared Documents/2. Documentación y procesos/12. Procesos automatizados/Liquidación gastos de viaje/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC104856B11F6C7C5ADE5903" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8265EB1E-C341-44CB-A65A-D5AA8D9A5672}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC104856B11F6C7C5ADE5903" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05101BA2-B6B1-4294-AF62-0E0EA8D638D3}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3300" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Empleado - Identificador</t>
   </si>
   <si>
     <t>Mail</t>
+  </si>
+  <si>
+    <t>ISMAEL_ASENJO</t>
+  </si>
+  <si>
+    <t>ismael.asenjo@stihl.es</t>
+  </si>
+  <si>
+    <t>ALTAMIRA</t>
+  </si>
+  <si>
+    <t>inaki.altamira@stihl.es</t>
+  </si>
+  <si>
+    <t>ORIOL_PINA</t>
+  </si>
+  <si>
+    <t>oriol.pina@stihl.es</t>
+  </si>
+  <si>
+    <t>TERESA_NIETO</t>
+  </si>
+  <si>
+    <t>teresa.nieto@stihl.es</t>
+  </si>
+  <si>
+    <t>BEGONA_RUIZ</t>
+  </si>
+  <si>
+    <t>begona.ruiz@stihl.es</t>
+  </si>
+  <si>
+    <t>ADOLFOCASASEMPERE</t>
+  </si>
+  <si>
+    <t>adolfo.casasempereblanquer@stihl.es</t>
+  </si>
+  <si>
+    <t>BERND_HULLERUM</t>
+  </si>
+  <si>
+    <t>bernd.hullerum@stihl.es</t>
+  </si>
+  <si>
+    <t>M_MARTINEZ</t>
+  </si>
+  <si>
+    <t>m.martinez@stihl.es</t>
+  </si>
+  <si>
+    <t>MARIO_BALTANAS</t>
+  </si>
+  <si>
+    <t>mario.baltanas@stihl.es</t>
+  </si>
+  <si>
+    <t>PEDRO_MOYANO</t>
+  </si>
+  <si>
+    <t>pedro.moyano@stihl.es</t>
+  </si>
+  <si>
+    <t>FERNANDO_BARRIO</t>
+  </si>
+  <si>
+    <t>fernando.barrio@stihl.es</t>
+  </si>
+  <si>
+    <t>BENJAMIN_MACKH</t>
+  </si>
+  <si>
+    <t>benjamin.mackh@stihl.es</t>
+  </si>
+  <si>
+    <t>ALVARO_LOPEZ</t>
+  </si>
+  <si>
+    <t>alvaro.lopez@stihl.es</t>
+  </si>
+  <si>
+    <t>ANA_SANCHEZ</t>
+  </si>
+  <si>
+    <t>ana.sanchez@stihl.es</t>
+  </si>
+  <si>
+    <t>ENRIQUE_ALONSO</t>
+  </si>
+  <si>
+    <t>enrique.alonso@stihl.es</t>
+  </si>
+  <si>
+    <t>ARANCHA_GANAN</t>
+  </si>
+  <si>
+    <t>arancha.ganan@stihl.es</t>
+  </si>
+  <si>
+    <t>JORGE_HEVIA</t>
+  </si>
+  <si>
+    <t>jorge.hevia@stihl.es</t>
+  </si>
+  <si>
+    <t>VICTOR_PRADA</t>
+  </si>
+  <si>
+    <t>victor.prada@stihl.es</t>
+  </si>
+  <si>
+    <t>RAQUEL_MUNOZ</t>
+  </si>
+  <si>
+    <t>raquel.munoz@stihl.es</t>
+  </si>
+  <si>
+    <t>JSANCHEZ</t>
+  </si>
+  <si>
+    <t>jsanchez@stihl.es</t>
+  </si>
+  <si>
+    <t>JOAQUIN_PORTILLO</t>
+  </si>
+  <si>
+    <t>joaquin.portillo@stihl.es</t>
+  </si>
+  <si>
+    <t>FERNANDO_ALVARO</t>
+  </si>
+  <si>
+    <t>fernando.alvarocastillo@stihl.es</t>
+  </si>
+  <si>
+    <t>ANDRES_LOPEZ</t>
+  </si>
+  <si>
+    <t>andres.lopez@stihl.es</t>
+  </si>
+  <si>
+    <t>JAVIER_SICILIA</t>
+  </si>
+  <si>
+    <t>javier.sicilia@stihl.es</t>
   </si>
   <si>
     <t>TONY_BLANCO</t>
@@ -54,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,10 +244,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,19 +509,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B25"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,12 +529,204 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -406,6 +738,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100812FB67C5E01F547A18D4A5FD6A8713D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9642c6788bad27e02d635fb107c9ae4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xmlns:ns3="d9b07192-7579-4291-b28e-58bbe42d995f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e8472eb4e8570153d151932821fc84c" ns2:_="" ns3:_="">
     <xsd:import namespace="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
@@ -640,24 +990,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d9b07192-7579-4291-b28e-58bbe42d995f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d3f5fe61-724b-4b88-a376-d24adb9ebb03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -668,39 +1000,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB358B33-21B5-44C6-8F12-C25C4054C5B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
-    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C25B787B-7428-43A6-BF3C-2BA84D875745}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C25B787B-7428-43A6-BF3C-2BA84D875745}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d3f5fe61-724b-4b88-a376-d24adb9ebb03"/>
-    <ds:schemaRef ds:uri="d9b07192-7579-4291-b28e-58bbe42d995f"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB358B33-21B5-44C6-8F12-C25C4054C5B3}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA831405-C37E-4AB9-AE22-2A9B47C9BFD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA831405-C37E-4AB9-AE22-2A9B47C9BFD1}"/>
 </file>
</xml_diff>